<commit_message>
Added test metadata for EGA/dbgap update.
</commit_message>
<xml_diff>
--- a/infrastructure_testing_files/test_metadata_hca_spreadsheet.xlsx
+++ b/infrastructure_testing_files/test_metadata_hca_spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/enrique/HumanCellAtlas/metadata-schema/infrastructure_testing_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C293890-1ABE-6841-98FF-326E62655B69}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5E90DD2-35C6-A448-932C-7FD43A069515}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="68800" windowHeight="26980" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22660" yWindow="460" windowWidth="40200" windowHeight="26860" firstSheet="9" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,6 @@
     <sheet name="Analysis protocol" sheetId="29" r:id="rId19"/>
     <sheet name="Analysis file" sheetId="30" r:id="rId20"/>
     <sheet name="Supplementary file" sheetId="20" r:id="rId21"/>
-    <sheet name="Schemas" sheetId="28" r:id="rId22"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -52,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10208" uniqueCount="2223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10184" uniqueCount="2199">
   <si>
     <t>PROJECT LABEL (Required)</t>
   </si>
@@ -6324,108 +6323,6 @@
     <t>ipsc_induction_protocol.reagents.kit_titer</t>
   </si>
   <si>
-    <t>Schemas</t>
-  </si>
-  <si>
-    <t>https://schema.integration.data.humancellatlas.org/type/protocol/sequencing/10.1.0/sequencing_protocol</t>
-  </si>
-  <si>
-    <t>https://schema.integration.data.humancellatlas.org/type/protocol/sequencing/6.2.0/library_preparation_protocol</t>
-  </si>
-  <si>
-    <t>https://schema.integration.data.humancellatlas.org/type/protocol/imaging/11.2.0/imaging_protocol</t>
-  </si>
-  <si>
-    <t>https://schema.integration.data.humancellatlas.org/type/protocol/imaging/2.2.0/imaging_preparation_protocol</t>
-  </si>
-  <si>
-    <t>https://schema.integration.data.humancellatlas.org/type/protocol/biomaterial_collection/3.2.0/ipsc_induction_protocol</t>
-  </si>
-  <si>
-    <t>https://schema.integration.data.humancellatlas.org/type/protocol/biomaterial_collection/3.1.0/enrichment_protocol</t>
-  </si>
-  <si>
-    <t>https://schema.integration.data.humancellatlas.org/type/protocol/biomaterial_collection/6.2.0/dissociation_protocol</t>
-  </si>
-  <si>
-    <t>https://schema.integration.data.humancellatlas.org/type/protocol/biomaterial_collection/2.2.0/differentiation_protocol</t>
-  </si>
-  <si>
-    <t>https://schema.integration.data.humancellatlas.org/type/protocol/biomaterial_collection/9.2.0/collection_protocol</t>
-  </si>
-  <si>
-    <t>https://schema.integration.data.humancellatlas.org/type/protocol/biomaterial_collection/2.1.0/aggregate_generation_protocol</t>
-  </si>
-  <si>
-    <t>https://schema.integration.data.humancellatlas.org/type/protocol/biomaterial/5.1.0/biomaterial_collection_protocol</t>
-  </si>
-  <si>
-    <t>https://schema.integration.data.humancellatlas.org/type/protocol/analysis/9.1.0/analysis_protocol</t>
-  </si>
-  <si>
-    <t>https://schema.integration.data.humancellatlas.org/type/protocol/7.1.0/protocol</t>
-  </si>
-  <si>
-    <t>https://schema.integration.data.humancellatlas.org/type/project/14.1.0/project</t>
-  </si>
-  <si>
-    <t>https://schema.integration.data.humancellatlas.org/type/process/sequencing/5.1.0/sequencing_process</t>
-  </si>
-  <si>
-    <t>https://schema.integration.data.humancellatlas.org/type/process/sequencing/5.1.0/library_preparation_process</t>
-  </si>
-  <si>
-    <t>https://schema.integration.data.humancellatlas.org/type/process/imaging/5.1.0/imaging_process</t>
-  </si>
-  <si>
-    <t>https://schema.integration.data.humancellatlas.org/type/process/biomaterial_collection/5.1.0/enrichment_process</t>
-  </si>
-  <si>
-    <t>https://schema.integration.data.humancellatlas.org/type/process/biomaterial_collection/5.1.0/dissociation_process</t>
-  </si>
-  <si>
-    <t>https://schema.integration.data.humancellatlas.org/type/process/biomaterial_collection/5.1.0/collection_process</t>
-  </si>
-  <si>
-    <t>https://schema.integration.data.humancellatlas.org/type/process/analysis/12.0.0/analysis_process</t>
-  </si>
-  <si>
-    <t>https://schema.integration.data.humancellatlas.org/type/process/9.2.0/process</t>
-  </si>
-  <si>
-    <t>https://schema.integration.data.humancellatlas.org/type/file/2.2.0/supplementary_file</t>
-  </si>
-  <si>
-    <t>https://schema.integration.data.humancellatlas.org/type/file/9.2.0/sequence_file</t>
-  </si>
-  <si>
-    <t>https://schema.integration.data.humancellatlas.org/type/file/3.2.0/reference_file</t>
-  </si>
-  <si>
-    <t>https://schema.integration.data.humancellatlas.org/type/file/2.2.0/image_file</t>
-  </si>
-  <si>
-    <t>https://schema.integration.data.humancellatlas.org/type/file/6.2.0/analysis_file</t>
-  </si>
-  <si>
-    <t>https://schema.integration.data.humancellatlas.org/type/biomaterial/10.4.0/specimen_from_organism</t>
-  </si>
-  <si>
-    <t>https://schema.integration.data.humancellatlas.org/type/biomaterial/11.3.0/organoid</t>
-  </si>
-  <si>
-    <t>https://schema.integration.data.humancellatlas.org/type/biomaterial/3.3.0/imaged_specimen</t>
-  </si>
-  <si>
-    <t>https://schema.integration.data.humancellatlas.org/type/biomaterial/15.5.0/donor_organism</t>
-  </si>
-  <si>
-    <t>https://schema.integration.data.humancellatlas.org/type/biomaterial/13.3.0/cell_suspension</t>
-  </si>
-  <si>
-    <t>https://schema.integration.data.humancellatlas.org/type/biomaterial/14.5.0/cell_line</t>
-  </si>
-  <si>
     <t>OBI:0000869</t>
   </si>
   <si>
@@ -6721,6 +6618,36 @@
   </si>
   <si>
     <t>analysis_protocol.protocol_core.protocol_name</t>
+  </si>
+  <si>
+    <t>project.ega_accessions</t>
+  </si>
+  <si>
+    <t>project.dbgap_accessions</t>
+  </si>
+  <si>
+    <t>EGA Study/Dataset Accession(s)</t>
+  </si>
+  <si>
+    <t>Enter any EGA study or dataset accessions that relate to the project. Should start with EGAD or EGAS, study accession preferred.</t>
+  </si>
+  <si>
+    <t>A list of European Genome phenome Archive dataset or study accessions.</t>
+  </si>
+  <si>
+    <t>dbGap Study Accession(s)</t>
+  </si>
+  <si>
+    <t>A list of database of Genotypes and Phenotypes (dbGaP) study accessions.</t>
+  </si>
+  <si>
+    <t>Enter any dbGaP study accessions that relate to this project. Should start with phs, can contain the specific version information.</t>
+  </si>
+  <si>
+    <t>EGAS00000000001||EGAD00000000002</t>
+  </si>
+  <si>
+    <t>phs001997.v1.p1||phs001836</t>
   </si>
 </sst>
 </file>
@@ -7170,10 +7097,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I37" sqref="I37"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7186,9 +7113,11 @@
     <col min="7" max="7" width="26.6640625" style="3" customWidth="1"/>
     <col min="8" max="8" width="25.6640625" style="3" customWidth="1"/>
     <col min="9" max="9" width="24.6640625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="29.83203125" customWidth="1"/>
+    <col min="11" max="11" width="40.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7216,8 +7145,14 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J1" s="1" t="s">
+        <v>2191</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>2194</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
@@ -7245,8 +7180,14 @@
       <c r="I2" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J2" s="2" t="s">
+        <v>2193</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>2195</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>18</v>
       </c>
@@ -7274,8 +7215,14 @@
       <c r="I3" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="J3" s="2" t="s">
+        <v>2192</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>2196</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="41" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -7303,8 +7250,14 @@
       <c r="I4" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J4" s="3" t="s">
+        <v>2189</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>2190</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>36</v>
       </c>
@@ -7316,8 +7269,10 @@
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>37</v>
       </c>
@@ -7344,6 +7299,12 @@
       </c>
       <c r="I6" t="s">
         <v>45</v>
+      </c>
+      <c r="J6" t="s">
+        <v>2197</v>
+      </c>
+      <c r="K6" t="s">
+        <v>2198</v>
       </c>
     </row>
   </sheetData>
@@ -8425,7 +8386,7 @@
         <v>970</v>
       </c>
       <c r="Y7" t="s">
-        <v>2154</v>
+        <v>2120</v>
       </c>
       <c r="Z7" t="s">
         <v>424</v>
@@ -8592,7 +8553,7 @@
         <v>974</v>
       </c>
       <c r="Y8" t="s">
-        <v>2155</v>
+        <v>2121</v>
       </c>
       <c r="Z8" t="s">
         <v>424</v>
@@ -8759,7 +8720,7 @@
         <v>978</v>
       </c>
       <c r="Y9" t="s">
-        <v>2156</v>
+        <v>2122</v>
       </c>
       <c r="Z9" t="s">
         <v>424</v>
@@ -8938,7 +8899,7 @@
         <v>984</v>
       </c>
       <c r="Y10" t="s">
-        <v>2157</v>
+        <v>2123</v>
       </c>
       <c r="Z10" t="s">
         <v>424</v>
@@ -9105,7 +9066,7 @@
         <v>988</v>
       </c>
       <c r="Y11" t="s">
-        <v>2158</v>
+        <v>2124</v>
       </c>
       <c r="Z11" t="s">
         <v>511</v>
@@ -9272,7 +9233,7 @@
         <v>992</v>
       </c>
       <c r="Y12" t="s">
-        <v>2159</v>
+        <v>2125</v>
       </c>
       <c r="Z12" t="s">
         <v>511</v>
@@ -9439,7 +9400,7 @@
         <v>996</v>
       </c>
       <c r="Y13" t="s">
-        <v>2160</v>
+        <v>2126</v>
       </c>
       <c r="Z13" t="s">
         <v>424</v>
@@ -9615,7 +9576,7 @@
         <v>1002</v>
       </c>
       <c r="Y14" t="s">
-        <v>2161</v>
+        <v>2127</v>
       </c>
       <c r="Z14" t="s">
         <v>424</v>
@@ -9782,7 +9743,7 @@
         <v>1006</v>
       </c>
       <c r="Y15" t="s">
-        <v>2162</v>
+        <v>2128</v>
       </c>
       <c r="Z15" t="s">
         <v>424</v>
@@ -9949,7 +9910,7 @@
         <v>1009</v>
       </c>
       <c r="Y16" t="s">
-        <v>2163</v>
+        <v>2129</v>
       </c>
       <c r="Z16" t="s">
         <v>424</v>
@@ -10116,7 +10077,7 @@
         <v>1012</v>
       </c>
       <c r="Y17" t="s">
-        <v>2164</v>
+        <v>2130</v>
       </c>
       <c r="Z17" t="s">
         <v>424</v>
@@ -10292,7 +10253,7 @@
         <v>1017</v>
       </c>
       <c r="Y18" t="s">
-        <v>2165</v>
+        <v>2131</v>
       </c>
       <c r="Z18" s="3" t="s">
         <v>424</v>
@@ -10459,7 +10420,7 @@
         <v>1021</v>
       </c>
       <c r="Y19" t="s">
-        <v>2166</v>
+        <v>2132</v>
       </c>
       <c r="Z19" s="3" t="s">
         <v>424</v>
@@ -10626,7 +10587,7 @@
         <v>1027</v>
       </c>
       <c r="Y20" t="s">
-        <v>2167</v>
+        <v>2133</v>
       </c>
       <c r="Z20" s="3" t="s">
         <v>424</v>
@@ -10793,7 +10754,7 @@
         <v>1033</v>
       </c>
       <c r="Y21" t="s">
-        <v>2168</v>
+        <v>2134</v>
       </c>
       <c r="Z21" s="3" t="s">
         <v>424</v>
@@ -10969,7 +10930,7 @@
         <v>1041</v>
       </c>
       <c r="Y22" t="s">
-        <v>2169</v>
+        <v>2135</v>
       </c>
       <c r="Z22" s="3" t="s">
         <v>424</v>
@@ -11136,7 +11097,7 @@
         <v>1047</v>
       </c>
       <c r="Y23" t="s">
-        <v>2170</v>
+        <v>2136</v>
       </c>
       <c r="Z23" s="3" t="s">
         <v>511</v>
@@ -11303,7 +11264,7 @@
         <v>1053</v>
       </c>
       <c r="Y24" t="s">
-        <v>2171</v>
+        <v>2137</v>
       </c>
       <c r="Z24" s="3" t="s">
         <v>511</v>
@@ -11470,7 +11431,7 @@
         <v>1059</v>
       </c>
       <c r="Y25" t="s">
-        <v>2172</v>
+        <v>2138</v>
       </c>
       <c r="Z25" s="3" t="s">
         <v>424</v>
@@ -11646,7 +11607,7 @@
         <v>1066</v>
       </c>
       <c r="Y26" t="s">
-        <v>2173</v>
+        <v>2139</v>
       </c>
       <c r="Z26" s="3" t="s">
         <v>424</v>
@@ -11813,7 +11774,7 @@
         <v>1072</v>
       </c>
       <c r="Y27" t="s">
-        <v>2174</v>
+        <v>2140</v>
       </c>
       <c r="Z27" s="3" t="s">
         <v>424</v>
@@ -11980,7 +11941,7 @@
         <v>1078</v>
       </c>
       <c r="Y28" t="s">
-        <v>2175</v>
+        <v>2141</v>
       </c>
       <c r="Z28" s="3" t="s">
         <v>424</v>
@@ -12147,7 +12108,7 @@
         <v>1084</v>
       </c>
       <c r="Y29" t="s">
-        <v>2176</v>
+        <v>2142</v>
       </c>
       <c r="Z29" s="3" t="s">
         <v>424</v>
@@ -12323,7 +12284,7 @@
         <v>1027</v>
       </c>
       <c r="Y30" t="s">
-        <v>2167</v>
+        <v>2133</v>
       </c>
       <c r="Z30" s="3" t="s">
         <v>424</v>
@@ -12371,7 +12332,7 @@
         <v>840</v>
       </c>
       <c r="AT30" s="3" t="s">
-        <v>2179</v>
+        <v>2145</v>
       </c>
       <c r="AU30" t="s">
         <v>441</v>
@@ -12490,7 +12451,7 @@
         <v>1033</v>
       </c>
       <c r="Y31" t="s">
-        <v>2168</v>
+        <v>2134</v>
       </c>
       <c r="Z31" s="3" t="s">
         <v>424</v>
@@ -12547,7 +12508,7 @@
         <v>840</v>
       </c>
       <c r="AT31" s="3" t="s">
-        <v>2180</v>
+        <v>2146</v>
       </c>
       <c r="AU31" t="s">
         <v>441</v>
@@ -12666,7 +12627,7 @@
         <v>1041</v>
       </c>
       <c r="Y32" t="s">
-        <v>2169</v>
+        <v>2135</v>
       </c>
       <c r="Z32" s="3" t="s">
         <v>424</v>
@@ -12714,7 +12675,7 @@
         <v>840</v>
       </c>
       <c r="AT32" s="3" t="s">
-        <v>2181</v>
+        <v>2147</v>
       </c>
       <c r="AU32" t="s">
         <v>441</v>
@@ -12833,7 +12794,7 @@
         <v>1047</v>
       </c>
       <c r="Y33" t="s">
-        <v>2170</v>
+        <v>2136</v>
       </c>
       <c r="Z33" s="3" t="s">
         <v>424</v>
@@ -12881,7 +12842,7 @@
         <v>840</v>
       </c>
       <c r="AT33" s="3" t="s">
-        <v>2182</v>
+        <v>2148</v>
       </c>
       <c r="AU33" t="s">
         <v>441</v>
@@ -13000,7 +12961,7 @@
         <v>1053</v>
       </c>
       <c r="Y34" t="s">
-        <v>2171</v>
+        <v>2137</v>
       </c>
       <c r="Z34" s="3" t="s">
         <v>424</v>
@@ -13048,7 +13009,7 @@
         <v>840</v>
       </c>
       <c r="AT34" s="3" t="s">
-        <v>2183</v>
+        <v>2149</v>
       </c>
       <c r="AU34" t="s">
         <v>441</v>
@@ -13167,7 +13128,7 @@
         <v>1059</v>
       </c>
       <c r="Y35" t="s">
-        <v>2172</v>
+        <v>2138</v>
       </c>
       <c r="Z35" s="3" t="s">
         <v>511</v>
@@ -13224,7 +13185,7 @@
         <v>840</v>
       </c>
       <c r="AT35" s="3" t="s">
-        <v>2184</v>
+        <v>2150</v>
       </c>
       <c r="AU35" t="s">
         <v>441</v>
@@ -13343,7 +13304,7 @@
         <v>1066</v>
       </c>
       <c r="Y36" t="s">
-        <v>2173</v>
+        <v>2139</v>
       </c>
       <c r="Z36" s="3" t="s">
         <v>511</v>
@@ -13391,7 +13352,7 @@
         <v>840</v>
       </c>
       <c r="AT36" s="3" t="s">
-        <v>2185</v>
+        <v>2151</v>
       </c>
       <c r="AU36" t="s">
         <v>441</v>
@@ -13510,7 +13471,7 @@
         <v>1072</v>
       </c>
       <c r="Y37" t="s">
-        <v>2174</v>
+        <v>2140</v>
       </c>
       <c r="Z37" s="3" t="s">
         <v>424</v>
@@ -13558,7 +13519,7 @@
         <v>840</v>
       </c>
       <c r="AT37" s="3" t="s">
-        <v>2186</v>
+        <v>2152</v>
       </c>
       <c r="AU37" t="s">
         <v>441</v>
@@ -13677,7 +13638,7 @@
         <v>1078</v>
       </c>
       <c r="Y38" t="s">
-        <v>2175</v>
+        <v>2141</v>
       </c>
       <c r="Z38" s="3" t="s">
         <v>424</v>
@@ -13725,7 +13686,7 @@
         <v>840</v>
       </c>
       <c r="AT38" s="3" t="s">
-        <v>2187</v>
+        <v>2153</v>
       </c>
       <c r="AU38" t="s">
         <v>441</v>
@@ -13844,7 +13805,7 @@
         <v>1084</v>
       </c>
       <c r="Y39" t="s">
-        <v>2176</v>
+        <v>2142</v>
       </c>
       <c r="Z39" s="3" t="s">
         <v>424</v>
@@ -13901,7 +13862,7 @@
         <v>840</v>
       </c>
       <c r="AT39" s="3" t="s">
-        <v>2188</v>
+        <v>2154</v>
       </c>
       <c r="AU39" t="s">
         <v>441</v>
@@ -14020,7 +13981,7 @@
         <v>1027</v>
       </c>
       <c r="Y40" t="s">
-        <v>2167</v>
+        <v>2133</v>
       </c>
       <c r="Z40" s="3" t="s">
         <v>424</v>
@@ -14068,7 +14029,7 @@
         <v>840</v>
       </c>
       <c r="AT40" s="3" t="s">
-        <v>2189</v>
+        <v>2155</v>
       </c>
       <c r="AU40" t="s">
         <v>441</v>
@@ -14187,7 +14148,7 @@
         <v>1033</v>
       </c>
       <c r="Y41" t="s">
-        <v>2168</v>
+        <v>2134</v>
       </c>
       <c r="Z41" s="3" t="s">
         <v>424</v>
@@ -14244,7 +14205,7 @@
         <v>840</v>
       </c>
       <c r="AT41" s="3" t="s">
-        <v>2190</v>
+        <v>2156</v>
       </c>
       <c r="AU41" t="s">
         <v>441</v>
@@ -14363,7 +14324,7 @@
         <v>1041</v>
       </c>
       <c r="Y42" t="s">
-        <v>2169</v>
+        <v>2135</v>
       </c>
       <c r="Z42" s="3" t="s">
         <v>424</v>
@@ -14411,7 +14372,7 @@
         <v>840</v>
       </c>
       <c r="AT42" s="3" t="s">
-        <v>2191</v>
+        <v>2157</v>
       </c>
       <c r="AU42" t="s">
         <v>441</v>
@@ -14530,7 +14491,7 @@
         <v>1047</v>
       </c>
       <c r="Y43" t="s">
-        <v>2170</v>
+        <v>2136</v>
       </c>
       <c r="Z43" s="3" t="s">
         <v>424</v>
@@ -14578,7 +14539,7 @@
         <v>840</v>
       </c>
       <c r="AT43" s="3" t="s">
-        <v>2192</v>
+        <v>2158</v>
       </c>
       <c r="AU43" t="s">
         <v>441</v>
@@ -18423,7 +18384,7 @@
         <v>1459</v>
       </c>
       <c r="BO6" t="s">
-        <v>2193</v>
+        <v>2159</v>
       </c>
       <c r="BP6" t="s">
         <v>1460</v>
@@ -18575,7 +18536,7 @@
         <v>1450</v>
       </c>
       <c r="AJ7" t="s">
-        <v>2154</v>
+        <v>2120</v>
       </c>
       <c r="AK7">
         <v>61</v>
@@ -18665,7 +18626,7 @@
         <v>1471</v>
       </c>
       <c r="BO7" s="3" t="s">
-        <v>2194</v>
+        <v>2160</v>
       </c>
       <c r="BP7" t="s">
         <v>1460</v>
@@ -18817,7 +18778,7 @@
         <v>1450</v>
       </c>
       <c r="AJ8" t="s">
-        <v>2155</v>
+        <v>2121</v>
       </c>
       <c r="AK8">
         <v>62</v>
@@ -18907,7 +18868,7 @@
         <v>1477</v>
       </c>
       <c r="BO8" s="3" t="s">
-        <v>2195</v>
+        <v>2161</v>
       </c>
       <c r="BP8" t="s">
         <v>1460</v>
@@ -19059,7 +19020,7 @@
         <v>1450</v>
       </c>
       <c r="AJ9" t="s">
-        <v>2156</v>
+        <v>2122</v>
       </c>
       <c r="AK9">
         <v>63</v>
@@ -19149,7 +19110,7 @@
         <v>1483</v>
       </c>
       <c r="BO9" s="3" t="s">
-        <v>2196</v>
+        <v>2162</v>
       </c>
       <c r="BP9" t="s">
         <v>1460</v>
@@ -19301,7 +19262,7 @@
         <v>1450</v>
       </c>
       <c r="AJ10" t="s">
-        <v>2157</v>
+        <v>2123</v>
       </c>
       <c r="AK10">
         <v>64</v>
@@ -19391,7 +19352,7 @@
         <v>1489</v>
       </c>
       <c r="BO10" s="3" t="s">
-        <v>2197</v>
+        <v>2163</v>
       </c>
       <c r="BP10" t="s">
         <v>1460</v>
@@ -19543,7 +19504,7 @@
         <v>1450</v>
       </c>
       <c r="AJ11" t="s">
-        <v>2158</v>
+        <v>2124</v>
       </c>
       <c r="AK11">
         <v>65</v>
@@ -19633,7 +19594,7 @@
         <v>1495</v>
       </c>
       <c r="BO11" s="3" t="s">
-        <v>2198</v>
+        <v>2164</v>
       </c>
       <c r="BP11" t="s">
         <v>1460</v>
@@ -19785,7 +19746,7 @@
         <v>1450</v>
       </c>
       <c r="AJ12" t="s">
-        <v>2159</v>
+        <v>2125</v>
       </c>
       <c r="AK12">
         <v>66</v>
@@ -19875,7 +19836,7 @@
         <v>1499</v>
       </c>
       <c r="BO12" s="3" t="s">
-        <v>2199</v>
+        <v>2165</v>
       </c>
       <c r="BP12" t="s">
         <v>1460</v>
@@ -20027,7 +19988,7 @@
         <v>1450</v>
       </c>
       <c r="AJ13" t="s">
-        <v>2160</v>
+        <v>2126</v>
       </c>
       <c r="AK13">
         <v>67</v>
@@ -20117,7 +20078,7 @@
         <v>1503</v>
       </c>
       <c r="BO13" s="3" t="s">
-        <v>2200</v>
+        <v>2166</v>
       </c>
       <c r="BP13" t="s">
         <v>1460</v>
@@ -20269,7 +20230,7 @@
         <v>1450</v>
       </c>
       <c r="AJ14" t="s">
-        <v>2161</v>
+        <v>2127</v>
       </c>
       <c r="AK14">
         <v>68</v>
@@ -20359,7 +20320,7 @@
         <v>1507</v>
       </c>
       <c r="BO14" s="3" t="s">
-        <v>2201</v>
+        <v>2167</v>
       </c>
       <c r="BP14" t="s">
         <v>1460</v>
@@ -20511,7 +20472,7 @@
         <v>1450</v>
       </c>
       <c r="AJ15" t="s">
-        <v>2162</v>
+        <v>2128</v>
       </c>
       <c r="AK15">
         <v>60</v>
@@ -20601,7 +20562,7 @@
         <v>1510</v>
       </c>
       <c r="BO15" s="3" t="s">
-        <v>2202</v>
+        <v>2168</v>
       </c>
       <c r="BP15" t="s">
         <v>1460</v>
@@ -20753,7 +20714,7 @@
         <v>1450</v>
       </c>
       <c r="AJ16" t="s">
-        <v>2163</v>
+        <v>2129</v>
       </c>
       <c r="AK16">
         <v>61</v>
@@ -20843,7 +20804,7 @@
         <v>1512</v>
       </c>
       <c r="BO16" s="3" t="s">
-        <v>2203</v>
+        <v>2169</v>
       </c>
       <c r="BP16" t="s">
         <v>1460</v>
@@ -20995,7 +20956,7 @@
         <v>1450</v>
       </c>
       <c r="AJ17" t="s">
-        <v>2164</v>
+        <v>2130</v>
       </c>
       <c r="AK17">
         <v>62</v>
@@ -21085,7 +21046,7 @@
         <v>1514</v>
       </c>
       <c r="BO17" s="3" t="s">
-        <v>2204</v>
+        <v>2170</v>
       </c>
       <c r="BP17" t="s">
         <v>1460</v>
@@ -21237,7 +21198,7 @@
         <v>1450</v>
       </c>
       <c r="AJ18" t="s">
-        <v>2165</v>
+        <v>2131</v>
       </c>
       <c r="AK18">
         <v>63</v>
@@ -21327,7 +21288,7 @@
         <v>1516</v>
       </c>
       <c r="BO18" s="3" t="s">
-        <v>2205</v>
+        <v>2171</v>
       </c>
       <c r="BP18" t="s">
         <v>1460</v>
@@ -21479,7 +21440,7 @@
         <v>1450</v>
       </c>
       <c r="AJ19" t="s">
-        <v>2166</v>
+        <v>2132</v>
       </c>
       <c r="AK19">
         <v>64</v>
@@ -21569,7 +21530,7 @@
         <v>1518</v>
       </c>
       <c r="BO19" s="3" t="s">
-        <v>2206</v>
+        <v>2172</v>
       </c>
       <c r="BP19" t="s">
         <v>1460</v>
@@ -21721,7 +21682,7 @@
         <v>1450</v>
       </c>
       <c r="AJ20" t="s">
-        <v>2167</v>
+        <v>2133</v>
       </c>
       <c r="AK20">
         <v>65</v>
@@ -21811,7 +21772,7 @@
         <v>1520</v>
       </c>
       <c r="BO20" s="3" t="s">
-        <v>2207</v>
+        <v>2173</v>
       </c>
       <c r="BP20" t="s">
         <v>1460</v>
@@ -21963,7 +21924,7 @@
         <v>1450</v>
       </c>
       <c r="AJ21" t="s">
-        <v>2168</v>
+        <v>2134</v>
       </c>
       <c r="AK21">
         <v>66</v>
@@ -22053,7 +22014,7 @@
         <v>1522</v>
       </c>
       <c r="BO21" s="3" t="s">
-        <v>2208</v>
+        <v>2174</v>
       </c>
       <c r="BP21" t="s">
         <v>1460</v>
@@ -22205,7 +22166,7 @@
         <v>1450</v>
       </c>
       <c r="AJ22" t="s">
-        <v>2169</v>
+        <v>2135</v>
       </c>
       <c r="AK22">
         <v>67</v>
@@ -22295,7 +22256,7 @@
         <v>1524</v>
       </c>
       <c r="BO22" s="3" t="s">
-        <v>2209</v>
+        <v>2175</v>
       </c>
       <c r="BP22" t="s">
         <v>1460</v>
@@ -22447,7 +22408,7 @@
         <v>1450</v>
       </c>
       <c r="AJ23" t="s">
-        <v>2170</v>
+        <v>2136</v>
       </c>
       <c r="AK23">
         <v>68</v>
@@ -22537,7 +22498,7 @@
         <v>1526</v>
       </c>
       <c r="BO23" s="3" t="s">
-        <v>2210</v>
+        <v>2176</v>
       </c>
       <c r="BP23" t="s">
         <v>1460</v>
@@ -22689,7 +22650,7 @@
         <v>1450</v>
       </c>
       <c r="AJ24" t="s">
-        <v>2171</v>
+        <v>2137</v>
       </c>
       <c r="AK24">
         <v>60</v>
@@ -22779,7 +22740,7 @@
         <v>1528</v>
       </c>
       <c r="BO24" s="3" t="s">
-        <v>2211</v>
+        <v>2177</v>
       </c>
       <c r="BP24" t="s">
         <v>1460</v>
@@ -22931,7 +22892,7 @@
         <v>1450</v>
       </c>
       <c r="AJ25" t="s">
-        <v>2172</v>
+        <v>2138</v>
       </c>
       <c r="AK25">
         <v>61</v>
@@ -23021,7 +22982,7 @@
         <v>1530</v>
       </c>
       <c r="BO25" s="3" t="s">
-        <v>2212</v>
+        <v>2178</v>
       </c>
       <c r="BP25" t="s">
         <v>1460</v>
@@ -23173,7 +23134,7 @@
         <v>1450</v>
       </c>
       <c r="AJ26" t="s">
-        <v>2173</v>
+        <v>2139</v>
       </c>
       <c r="AK26">
         <v>62</v>
@@ -23263,7 +23224,7 @@
         <v>1532</v>
       </c>
       <c r="BO26" s="3" t="s">
-        <v>2213</v>
+        <v>2179</v>
       </c>
       <c r="BP26" t="s">
         <v>1460</v>
@@ -23415,7 +23376,7 @@
         <v>1450</v>
       </c>
       <c r="AJ27" t="s">
-        <v>2174</v>
+        <v>2140</v>
       </c>
       <c r="AK27">
         <v>63</v>
@@ -23505,7 +23466,7 @@
         <v>1534</v>
       </c>
       <c r="BO27" s="3" t="s">
-        <v>2214</v>
+        <v>2180</v>
       </c>
       <c r="BP27" t="s">
         <v>1460</v>
@@ -23657,7 +23618,7 @@
         <v>1450</v>
       </c>
       <c r="AJ28" t="s">
-        <v>2175</v>
+        <v>2141</v>
       </c>
       <c r="AK28">
         <v>64</v>
@@ -23747,7 +23708,7 @@
         <v>1536</v>
       </c>
       <c r="BO28" s="3" t="s">
-        <v>2215</v>
+        <v>2181</v>
       </c>
       <c r="BP28" t="s">
         <v>1460</v>
@@ -23899,7 +23860,7 @@
         <v>1450</v>
       </c>
       <c r="AJ29" t="s">
-        <v>2176</v>
+        <v>2142</v>
       </c>
       <c r="AK29">
         <v>65</v>
@@ -23989,7 +23950,7 @@
         <v>1538</v>
       </c>
       <c r="BO29" s="3" t="s">
-        <v>2216</v>
+        <v>2182</v>
       </c>
       <c r="BP29" t="s">
         <v>1460</v>
@@ -24801,7 +24762,7 @@
         <v>1672</v>
       </c>
       <c r="L6" s="6" t="s">
-        <v>2124</v>
+        <v>2090</v>
       </c>
       <c r="M6" s="6" t="s">
         <v>1672</v>
@@ -24956,7 +24917,7 @@
         <v>1672</v>
       </c>
       <c r="L7" s="6" t="s">
-        <v>2124</v>
+        <v>2090</v>
       </c>
       <c r="M7" s="6" t="s">
         <v>1672</v>
@@ -25111,7 +25072,7 @@
         <v>1672</v>
       </c>
       <c r="L8" s="6" t="s">
-        <v>2124</v>
+        <v>2090</v>
       </c>
       <c r="M8" s="6" t="s">
         <v>1672</v>
@@ -25266,7 +25227,7 @@
         <v>1672</v>
       </c>
       <c r="L9" s="6" t="s">
-        <v>2124</v>
+        <v>2090</v>
       </c>
       <c r="M9" s="6" t="s">
         <v>1672</v>
@@ -25421,7 +25382,7 @@
         <v>1672</v>
       </c>
       <c r="L10" s="6" t="s">
-        <v>2124</v>
+        <v>2090</v>
       </c>
       <c r="M10" s="6" t="s">
         <v>1672</v>
@@ -26623,7 +26584,7 @@
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>2218</v>
+        <v>2184</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>1808</v>
@@ -26638,7 +26599,7 @@
         <v>1811</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>2219</v>
+        <v>2185</v>
       </c>
       <c r="H9" s="3">
         <v>1</v>
@@ -35708,7 +35669,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5C087ED-AA0C-7842-A521-494DCB0E36A7}">
   <dimension ref="A1:R7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4:B4"/>
     </sheetView>
   </sheetViews>
@@ -35735,13 +35696,13 @@
   <sheetData>
     <row r="1" spans="1:18" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>2149</v>
+        <v>2115</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>2150</v>
+        <v>2116</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2148</v>
+        <v>2114</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>118</v>
@@ -35750,12 +35711,12 @@
         <v>547</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>2151</v>
+        <v>2117</v>
       </c>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1" t="s">
-        <v>2152</v>
+        <v>2118</v>
       </c>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
@@ -35825,31 +35786,31 @@
     </row>
     <row r="4" spans="1:18" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>2221</v>
+        <v>2187</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>2222</v>
+        <v>2188</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>2125</v>
+        <v>2091</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>2126</v>
+        <v>2092</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>2127</v>
+        <v>2093</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>2128</v>
+        <v>2094</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>2129</v>
+        <v>2095</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>2130</v>
+        <v>2096</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>2137</v>
+        <v>2103</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -35900,7 +35861,7 @@
         <v>601</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>2146</v>
+        <v>2112</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
@@ -35929,7 +35890,7 @@
         <v>601</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>2147</v>
+        <v>2113</v>
       </c>
     </row>
   </sheetData>
@@ -36264,7 +36225,7 @@
         <v>1765</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>2149</v>
+        <v>2115</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>1539</v>
@@ -36471,22 +36432,22 @@
     </row>
     <row r="4" spans="1:26" ht="43" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>2131</v>
+        <v>2097</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>2132</v>
+        <v>2098</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>2133</v>
+        <v>2099</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>2134</v>
+        <v>2100</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>2135</v>
+        <v>2101</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>2136</v>
+        <v>2102</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>1796</v>
@@ -36579,34 +36540,34 @@
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>2139</v>
+        <v>2105</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>2217</v>
+        <v>2183</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>2141</v>
+        <v>2107</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>2142</v>
+        <v>2108</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>2140</v>
+        <v>2106</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>2220</v>
+        <v>2186</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>1752</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>2143</v>
+        <v>2109</v>
       </c>
       <c r="J6" s="3" t="s">
         <v>1752</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>2145</v>
+        <v>2111</v>
       </c>
       <c r="L6" s="3" t="s">
         <v>1815</v>
@@ -36656,22 +36617,22 @@
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>2138</v>
+        <v>2104</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>2217</v>
+        <v>2183</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>2141</v>
+        <v>2107</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>2142</v>
+        <v>2108</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>2140</v>
+        <v>2106</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>2153</v>
+        <v>2119</v>
       </c>
       <c r="H7" s="3" t="s">
         <v>1762</v>
@@ -36683,7 +36644,7 @@
         <v>1762</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>2144</v>
+        <v>2110</v>
       </c>
       <c r="L7" s="3" t="s">
         <v>1815</v>
@@ -37141,7 +37102,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:W14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="M6" sqref="M6:N6"/>
     </sheetView>
   </sheetViews>
@@ -37501,10 +37462,10 @@
         <v>1817</v>
       </c>
       <c r="M6" s="11" t="s">
-        <v>2177</v>
+        <v>2143</v>
       </c>
       <c r="N6" s="11" t="s">
-        <v>2178</v>
+        <v>2144</v>
       </c>
       <c r="O6">
         <v>1</v>
@@ -37568,198 +37529,6 @@
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
-  <dimension ref="A1:A34"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="8.83203125" style="3" customWidth="1"/>
-    <col min="2" max="16384" width="8.83203125" style="3"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>2090</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
-        <v>2091</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
-        <v>2092</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
-        <v>2093</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
-        <v>2094</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
-        <v>2095</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
-        <v>2096</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
-        <v>2097</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
-        <v>2098</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
-        <v>2099</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="s">
-        <v>2100</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" s="5" t="s">
-        <v>2101</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13" s="5" t="s">
-        <v>2102</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A14" s="5" t="s">
-        <v>2103</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A15" s="5" t="s">
-        <v>2104</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A16" s="5" t="s">
-        <v>2105</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="5" t="s">
-        <v>2106</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="5" t="s">
-        <v>2107</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="5" t="s">
-        <v>2108</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" s="5" t="s">
-        <v>2109</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" s="5" t="s">
-        <v>2110</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" s="5" t="s">
-        <v>2111</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" s="5" t="s">
-        <v>2112</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" s="5" t="s">
-        <v>2113</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" s="5" t="s">
-        <v>2114</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" s="5" t="s">
-        <v>2115</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" s="5" t="s">
-        <v>2116</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28" s="5" t="s">
-        <v>2117</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A29" s="5" t="s">
-        <v>2118</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A30" s="5" t="s">
-        <v>2119</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A31" s="5" t="s">
-        <v>2120</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A32" s="5" t="s">
-        <v>2121</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" s="5" t="s">
-        <v>2122</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34" s="5" t="s">
-        <v>2123</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-1B00-000000000000}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>